<commit_message>
make XLSX file more interesting and shorter
before:
Formulas: [ [ 1, '=NOW()' ], [ 'a', '=1+2' ], [ '=TODAY()', '=A3' ] ]
Values:   [ [ 1, 44879.922650463 ], [ 'a', 3 ], [ 44879, 44879 ] ]

after:
Formulas: [ [ 1, '=A1+2' ], [ '=TODAY()', '=TEXT(A2,"YYYY-MM-DD")' ] ]
Values:   [ [ 1, 3 ], [ 44879, '2022-11-14' ] ]
</commit_message>
<xml_diff>
--- a/read-excel-file/sample_file.xlsx
+++ b/read-excel-file/sample_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakub\HotRepos\hyperformula-demos\read-excel-file\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/warp/www/hyperformula-demos/read-excel-file/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5397BCC-00AB-4659-8E1D-525E3913B016}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE3BD93-EF0C-1F40-9068-B74CB83E13BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6B37ABA7-C604-49FF-9C2F-D6A5A15C5D52}"/>
+    <workbookView xWindow="25740" yWindow="19460" windowWidth="25180" windowHeight="9060" xr2:uid="{6B37ABA7-C604-49FF-9C2F-D6A5A15C5D52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,11 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>a</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -77,7 +73,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,44 +388,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE1B462B-98A8-4A93-BB05-06EE1298C669}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" s="2">
-        <f ca="1">NOW()</f>
-        <v>44873.568243518515</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <f>1+2</f>
+        <f>A1+2</f>
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <f ca="1">TODAY()</f>
-        <v>44873</v>
+        <v>44879</v>
       </c>
-      <c r="B3" s="1">
-        <f ca="1">A3</f>
-        <v>44873</v>
+      <c r="B2" s="1" t="str">
+        <f ca="1">TEXT(A2,"YYYY-MM-DD")</f>
+        <v>2022-11-14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>